<commit_message>
Génération du template BDS
</commit_message>
<xml_diff>
--- a/Documentation/Documents/planningTaboada.xlsx
+++ b/Documentation/Documents/planningTaboada.xlsx
@@ -1188,10 +1188,10 @@
   </sheetPr>
   <dimension ref="A2:CO33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6735"/>
-      <selection activeCell="G11" sqref="G11"/>
-      <selection pane="topRight" activeCell="AD38" sqref="AD38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="5325" topLeftCell="I1" activePane="topRight"/>
+      <selection activeCell="D15" sqref="D15"/>
+      <selection pane="topRight" activeCell="AL36" sqref="AL36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1208,7 +1208,7 @@
     <col min="29" max="70" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:93" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:93" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
         <v>27</v>
       </c>
@@ -1218,7 +1218,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="2:93" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:93" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -1233,7 +1233,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="42">
-        <v>42857</v>
+        <v>42860</v>
       </c>
       <c r="O3" s="42"/>
       <c r="Q3" s="9"/>
@@ -1261,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:93" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:93" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -1274,12 +1274,12 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:93" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.3">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:93" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:93" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="17" t="s">
         <v>10</v>
@@ -1303,7 +1303,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:93" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:93" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1592,7 +1592,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
       <c r="B9" s="29" t="s">
         <v>14</v>
       </c>
@@ -1603,7 +1604,7 @@
       <c r="G9" s="34"/>
       <c r="H9" s="35"/>
     </row>
-    <row r="10" spans="2:93" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:93" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>33</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>15</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>16</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:93" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:93" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>18</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:93" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>19</v>
       </c>
@@ -1839,6 +1840,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
       <c r="B21" s="29" t="s">
         <v>21</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>42856</v>
       </c>
       <c r="D22" s="24">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E22" s="21">
         <f t="shared" ref="E22:F24" si="3">C22</f>
@@ -1865,7 +1867,7 @@
       </c>
       <c r="F22" s="14">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15">
         <v>0.6</v>
@@ -1879,7 +1881,7 @@
         <v>42856</v>
       </c>
       <c r="D23" s="24">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" ref="E23" si="4">C23</f>
@@ -1887,7 +1889,7 @@
       </c>
       <c r="F23" s="14">
         <f t="shared" ref="F23" si="5">D23</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G23" s="15">
         <v>0.4</v>
@@ -1899,18 +1901,18 @@
       </c>
       <c r="C24" s="25">
         <f>C23+D23+2</f>
-        <v>42870</v>
+        <v>42877</v>
       </c>
       <c r="D24" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E24" s="21">
         <f t="shared" si="3"/>
-        <v>42870</v>
+        <v>42877</v>
       </c>
       <c r="F24" s="14">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G24" s="15">
         <v>0</v>
@@ -1921,14 +1923,14 @@
         <v>32</v>
       </c>
       <c r="C25" s="25">
-        <v>42863</v>
+        <v>42870</v>
       </c>
       <c r="D25" s="24">
         <v>12</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" ref="E25:E33" si="6">C25</f>
-        <v>42863</v>
+        <v>42870</v>
       </c>
       <c r="F25" s="14">
         <f>D25</f>
@@ -2047,7 +2049,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="25"/>
       <c r="D33" s="24"/>

</xml_diff>